<commit_message>
Multi Input Version Working
</commit_message>
<xml_diff>
--- a/Logger V1.0/12_03/Logger.xlsx
+++ b/Logger V1.0/12_03/Logger.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A55FFA4-8A3B-44BC-81DF-4A4B8A6C5FFB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DA594C-9412-4ADA-9383-B3353AE2DD6D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="59">
   <si>
     <t>Circuit Testing</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>Two Diodes (Par and Ser), Perfect! More voltage maybe (Z not so much)</t>
+  </si>
+  <si>
+    <t>4.01</t>
   </si>
 </sst>
 </file>
@@ -267,7 +270,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -330,14 +333,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="27">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -488,15 +485,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -543,28 +531,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -656,7 +622,7 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -706,6 +672,84 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="18" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="19" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="21" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="16" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -741,103 +785,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="24" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="24" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="24" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="25" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="10" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="17" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="24" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="24" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1126,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,90 +1093,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="43"/>
-      <c r="B1" s="19" t="s">
+      <c r="A1" s="29"/>
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="20"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="48"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="44"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="22"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="50"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="24"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="52"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="27" t="s">
+      <c r="A4" s="30"/>
+      <c r="B4" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="53" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="44"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="14" t="s">
         <v>14</v>
       </c>
@@ -1253,7 +1200,7 @@
       <c r="H6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="45" t="s">
         <v>10</v>
       </c>
       <c r="J6" s="9" t="s">
@@ -1261,7 +1208,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1275,23 +1222,23 @@
         <v>6.9999999999999998E-9</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" ref="F7:F31" si="0">1/(2*PI()*D7*E7)</f>
+        <f t="shared" ref="F7:F23" si="0">1/(2*PI()*D7*E7)</f>
         <v>22.736420441699334</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" ref="G7:G31" si="1">D7*E7</f>
+        <f t="shared" ref="G7:G23" si="1">D7*E7</f>
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="18"/>
+      <c r="I7" s="46"/>
       <c r="J7" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1315,13 +1262,13 @@
       <c r="H8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="18"/>
+      <c r="I8" s="46"/>
       <c r="J8" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
@@ -1345,13 +1292,13 @@
       <c r="H9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="18"/>
+      <c r="I9" s="46"/>
       <c r="J9" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1375,13 +1322,13 @@
       <c r="H10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="18"/>
+      <c r="I10" s="46"/>
       <c r="J10" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1405,13 +1352,13 @@
       <c r="H11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="18"/>
+      <c r="I11" s="46"/>
       <c r="J11" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1435,13 +1382,13 @@
       <c r="H12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="18"/>
+      <c r="I12" s="46"/>
       <c r="J12" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1463,13 +1410,13 @@
       <c r="H13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="18"/>
+      <c r="I13" s="46"/>
       <c r="J13" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
@@ -1493,13 +1440,13 @@
       <c r="H14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="18"/>
+      <c r="I14" s="46"/>
       <c r="J14" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
@@ -1520,48 +1467,48 @@
         <f t="shared" si="1"/>
         <v>0.10340000000000001</v>
       </c>
-      <c r="H15" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="34" t="s">
+      <c r="H15" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="46"/>
+      <c r="J15" s="22" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
-      <c r="B16" s="30" t="s">
+      <c r="A16" s="30"/>
+      <c r="B16" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="18">
         <v>2</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="19">
         <v>1000000</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="20">
         <v>2.1999999999999998E-8</v>
       </c>
-      <c r="F16" s="31">
+      <c r="F16" s="19">
         <f t="shared" si="0"/>
         <v>7.2343155950861533</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="19">
         <f t="shared" si="1"/>
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="H16" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="41" t="s">
+      <c r="H16" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="J16" s="35" t="s">
+      <c r="J16" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="6" t="s">
         <v>34</v>
       </c>
@@ -1585,13 +1532,13 @@
       <c r="H17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I17" s="42"/>
-      <c r="J17" s="36" t="s">
+      <c r="I17" s="38"/>
+      <c r="J17" s="24" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="6" t="s">
         <v>36</v>
       </c>
@@ -1615,13 +1562,13 @@
       <c r="H18" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I18" s="42"/>
-      <c r="J18" s="37" t="s">
+      <c r="I18" s="38"/>
+      <c r="J18" s="25" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="6" t="s">
         <v>38</v>
       </c>
@@ -1645,13 +1592,13 @@
       <c r="H19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="37" t="s">
+      <c r="I19" s="38"/>
+      <c r="J19" s="25" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="6" t="s">
         <v>41</v>
       </c>
@@ -1675,13 +1622,13 @@
       <c r="H20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I20" s="42"/>
-      <c r="J20" s="38" t="s">
+      <c r="I20" s="38"/>
+      <c r="J20" s="26" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="6" t="s">
         <v>43</v>
       </c>
@@ -1705,13 +1652,13 @@
       <c r="H21" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I21" s="42"/>
-      <c r="J21" s="39" t="s">
+      <c r="I21" s="38"/>
+      <c r="J21" s="27" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="6" t="s">
         <v>45</v>
       </c>
@@ -1735,13 +1682,13 @@
       <c r="H22" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="42"/>
-      <c r="J22" s="39" t="s">
+      <c r="I22" s="38"/>
+      <c r="J22" s="27" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="30"/>
       <c r="B23" s="6" t="s">
         <v>47</v>
       </c>
@@ -1765,46 +1712,46 @@
       <c r="H23" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I23" s="42"/>
-      <c r="J23" s="40" t="s">
+      <c r="I23" s="38"/>
+      <c r="J23" s="28" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
-      <c r="B24" s="48" t="s">
+      <c r="A24" s="30"/>
+      <c r="B24" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="49">
+      <c r="C24" s="33">
         <v>5</v>
       </c>
-      <c r="D24" s="50">
+      <c r="D24" s="34">
         <v>1000000</v>
       </c>
-      <c r="E24" s="50">
+      <c r="E24" s="34">
         <v>4.0000000000000002E-9</v>
       </c>
-      <c r="F24" s="50">
+      <c r="F24" s="34">
         <f>1/(2*PI()*D24*E24)</f>
         <v>39.78873577297383</v>
       </c>
-      <c r="G24" s="50">
+      <c r="G24" s="34">
         <f>D24*E24</f>
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="H24" s="51" t="s">
-        <v>12</v>
-      </c>
-      <c r="I24" s="52" t="s">
+      <c r="H24" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="J24" s="60" t="s">
+      <c r="J24" s="41" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
-      <c r="B25" s="53" t="s">
+      <c r="A25" s="30"/>
+      <c r="B25" s="36" t="s">
         <v>50</v>
       </c>
       <c r="C25" s="1">
@@ -1817,22 +1764,22 @@
         <v>4.0000000000000002E-9</v>
       </c>
       <c r="F25" s="2">
-        <f t="shared" ref="F25:F33" si="2">1/(2*PI()*D25*E25)</f>
+        <f t="shared" ref="F25:F30" si="2">1/(2*PI()*D25*E25)</f>
         <v>39.78873577297383</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" ref="G25:G33" si="3">D25*E25</f>
+        <f t="shared" ref="G25:G30" si="3">D25*E25</f>
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="54"/>
-      <c r="J25" s="61"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="42"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
-      <c r="B26" s="53" t="s">
+      <c r="A26" s="30"/>
+      <c r="B26" s="36" t="s">
         <v>52</v>
       </c>
       <c r="C26" s="1">
@@ -1855,14 +1802,14 @@
       <c r="H26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I26" s="54"/>
-      <c r="J26" s="62" t="s">
+      <c r="I26" s="40"/>
+      <c r="J26" s="43" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
-      <c r="B27" s="53" t="s">
+      <c r="A27" s="30"/>
+      <c r="B27" s="36" t="s">
         <v>53</v>
       </c>
       <c r="C27" s="1">
@@ -1885,12 +1832,12 @@
       <c r="H27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I27" s="54"/>
-      <c r="J27" s="62"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="43"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
-      <c r="B28" s="53" t="s">
+      <c r="A28" s="30"/>
+      <c r="B28" s="36" t="s">
         <v>55</v>
       </c>
       <c r="C28" s="1">
@@ -1913,14 +1860,14 @@
       <c r="H28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I28" s="54"/>
-      <c r="J28" s="63" t="s">
+      <c r="I28" s="40"/>
+      <c r="J28" s="44" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
-      <c r="B29" s="53" t="s">
+    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="30"/>
+      <c r="B29" s="36" t="s">
         <v>56</v>
       </c>
       <c r="C29" s="4">
@@ -1943,186 +1890,343 @@
       <c r="H29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="54"/>
-      <c r="J29" s="63"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
-      <c r="B30" s="53" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="1">
-        <v>2</v>
-      </c>
-      <c r="D30" s="2">
-        <v>680000</v>
-      </c>
-      <c r="E30" s="2">
-        <v>2.2000000000000001E-7</v>
-      </c>
-      <c r="F30" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0638699404538459</v>
-      </c>
-      <c r="G30" s="2">
-        <f t="shared" si="3"/>
-        <v>0.14960000000000001</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I30" s="54"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="14">
+        <v>5</v>
+      </c>
+      <c r="D30" s="15">
+        <v>1000000</v>
+      </c>
+      <c r="E30" s="15">
+        <v>2.1999999999999998E-8</v>
+      </c>
+      <c r="F30" s="15">
+        <f>1/(2*PI()*D30*E30)</f>
+        <v>7.2343155950861533</v>
+      </c>
+      <c r="G30" s="15">
+        <f>D30*E30</f>
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="44"/>
-      <c r="B31" s="53" t="s">
-        <v>24</v>
+      <c r="A31" s="30"/>
+      <c r="B31" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C31" s="1">
         <v>5</v>
       </c>
       <c r="D31" s="2">
-        <v>680000</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>12</v>
+        <v>1000000</v>
+      </c>
+      <c r="E31" s="2">
+        <v>6.9999999999999998E-9</v>
       </c>
       <c r="F31" s="2">
-        <v>0</v>
+        <f t="shared" ref="F31:F39" si="4">1/(2*PI()*D31*E31)</f>
+        <v>22.736420441699334</v>
       </c>
       <c r="G31" s="2">
-        <v>0</v>
+        <f t="shared" ref="G31:G39" si="5">D31*E31</f>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I31" s="54"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="10" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="44"/>
-      <c r="B32" s="53" t="s">
-        <v>27</v>
+      <c r="A32" s="30"/>
+      <c r="B32" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C32" s="1">
         <v>5</v>
       </c>
       <c r="D32" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2.0000000000000001E-9</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="4"/>
+        <v>79.57747154594766</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="5"/>
+        <v>2E-3</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" s="46"/>
+      <c r="J32" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="30"/>
+      <c r="B33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="1">
+        <v>5</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="E33" s="2">
+        <v>4.0000000000000001E-8</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" si="4"/>
+        <v>3.9788735772973833</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="5"/>
+        <v>0.04</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I33" s="46"/>
+      <c r="J33" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="30"/>
+      <c r="B34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="E34" s="2">
+        <v>2.2000000000000001E-7</v>
+      </c>
+      <c r="F34" s="2">
+        <f t="shared" si="4"/>
+        <v>0.72343155950861526</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="5"/>
+        <v>0.22</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I34" s="46"/>
+      <c r="J34" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="30"/>
+      <c r="B35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="4">
+        <v>5</v>
+      </c>
+      <c r="D35" s="2">
         <v>680000</v>
       </c>
-      <c r="E32" s="2">
-        <v>8.4999999999999994E-8</v>
-      </c>
-      <c r="F32" s="2">
-        <f t="shared" ref="F32:F33" si="4">1/(2*PI()*D32*E32)</f>
-        <v>2.7535457282334841</v>
-      </c>
-      <c r="G32" s="2">
-        <f t="shared" ref="G32:G33" si="5">D32*E32</f>
-        <v>5.7799999999999997E-2</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I32" s="54"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
-      <c r="B33" s="55" t="s">
+      <c r="E35" s="2">
+        <v>2.1999999999999998E-8</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" si="4"/>
+        <v>10.63869940453846</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="5"/>
+        <v>1.4959999999999999E-2</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" s="46"/>
+      <c r="J35" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="30"/>
+      <c r="B36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="1">
+        <v>2</v>
+      </c>
+      <c r="D36" s="2">
+        <v>680000</v>
+      </c>
+      <c r="E36" s="2">
+        <v>2.2000000000000001E-7</v>
+      </c>
+      <c r="F36" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0638699404538459</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="5"/>
+        <v>0.14960000000000001</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" s="46"/>
+      <c r="J36" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="30"/>
+      <c r="B37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="1">
+        <v>5</v>
+      </c>
+      <c r="D37" s="2">
+        <v>680000</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="46"/>
+      <c r="J37" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="30"/>
+      <c r="B38" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="1">
+        <v>5</v>
+      </c>
+      <c r="D38" s="2">
+        <v>680000</v>
+      </c>
+      <c r="E38" s="2">
+        <v>8.4999999999999996E-10</v>
+      </c>
+      <c r="F38" s="2">
+        <f t="shared" ref="F38:F39" si="6">1/(2*PI()*D38*E38)</f>
+        <v>275.35457282334835</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" ref="G38:G39" si="7">D38*E38</f>
+        <v>5.7799999999999995E-4</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="46"/>
+      <c r="J38" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="30"/>
+      <c r="B39" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="56">
+      <c r="C39" s="1">
         <v>3</v>
       </c>
-      <c r="D33" s="57">
+      <c r="D39" s="2">
         <v>470000</v>
       </c>
-      <c r="E33" s="57">
+      <c r="E39" s="2">
         <v>2.2000000000000001E-7</v>
       </c>
-      <c r="F33" s="57">
-        <f t="shared" si="4"/>
+      <c r="F39" s="2">
+        <f t="shared" si="6"/>
         <v>1.5392160840608833</v>
       </c>
-      <c r="G33" s="57">
-        <f t="shared" si="5"/>
+      <c r="G39" s="2">
+        <f t="shared" si="7"/>
         <v>0.10340000000000001</v>
       </c>
-      <c r="H33" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="I33" s="59"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="44"/>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="46"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="44"/>
-      <c r="B35" s="47"/>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="44"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="44"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="44"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="44"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="44"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="44"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="44"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="44"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="44"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="44"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="44"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="44"/>
+      <c r="H39" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="46"/>
+      <c r="J39" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="30"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="30"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="30"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="30"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="30"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="30"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="30"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="30"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="30"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="45"/>
+      <c r="A49" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="I16:I23"/>
-    <mergeCell ref="I24:I33"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="J28:J29"/>
+  <mergeCells count="18">
+    <mergeCell ref="I24:I29"/>
+    <mergeCell ref="I30:I39"/>
     <mergeCell ref="I6:I15"/>
     <mergeCell ref="B1:K2"/>
     <mergeCell ref="B3:K3"/>
@@ -2135,6 +2239,10 @@
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I16:I23"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="J28:J29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>